<commit_message>
new mechs and exps
</commit_message>
<xml_diff>
--- a/lib/jobs/c3h8_rcm_dames_2016.xlsx
+++ b/lib/jobs/c3h8_rcm_dames_2016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mulvihcr/PycharmProjects/pythonProject/mechsimulator/lib/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4428D2C8-743D-EF46-A143-2B3564876E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CECF145-25DC-8B4E-8D56-5758CE5AD878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44400" yWindow="13320" windowWidth="21440" windowHeight="11640" activeTab="1" xr2:uid="{E67FD926-F6F9-4D40-89D7-F9619D8CC074}"/>
+    <workbookView xWindow="41620" yWindow="12460" windowWidth="21440" windowHeight="11640" activeTab="1" xr2:uid="{E67FD926-F6F9-4D40-89D7-F9619D8CC074}"/>
   </bookViews>
   <sheets>
     <sheet name="exp" sheetId="1" r:id="rId1"/>
@@ -65,16 +65,16 @@
     <t>outcome</t>
   </si>
   <si>
-    <t>dames_2016_c3h8_rcm_idt_phi05.xlsx</t>
-  </si>
-  <si>
     <t>nuig1.2.csv</t>
   </si>
   <si>
-    <t>nuig1.2_reduced.cti</t>
-  </si>
-  <si>
-    <t>NUIG1.2, reduced</t>
+    <t>dames_2016_c3h8_rcm_idt_phi1.xlsx</t>
+  </si>
+  <si>
+    <t>nuig1.2_reduced5.cti</t>
+  </si>
+  <si>
+    <t>NUIG1.2, reduced 5</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,7 +453,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -475,14 +475,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -501,7 +501,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>

</xml_diff>